<commit_message>
subject chosen in directWord
</commit_message>
<xml_diff>
--- a/src/main/resources/static/import_temp/template.xlsx
+++ b/src/main/resources/static/import_temp/template.xlsx
@@ -1,39 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11008"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/23Fall/JAVA/finalProj/KaskadeMindBank/src/main/resources/static/import_temp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B830DD-F556-E24C-B33E-285AF4CFCFB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D32F3C-CFAA-9245-A509-5A0A9BF66516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9180" yWindow="2440" windowWidth="28260" windowHeight="17320" activeTab="2" xr2:uid="{54A98207-D246-064D-A28A-1B5B6DDC0A93}"/>
+    <workbookView xWindow="2960" yWindow="660" windowWidth="22500" windowHeight="13700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fill" sheetId="1" r:id="rId1"/>
     <sheet name="Judge" sheetId="2" r:id="rId2"/>
     <sheet name="Select" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -41,79 +25,60 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>主题</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>题目描述</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>答案</t>
+  </si>
+  <si>
+    <t>表格测试</t>
+  </si>
+  <si>
+    <t>小鱼姓什么</t>
+  </si>
+  <si>
+    <t>姓王！</t>
+  </si>
+  <si>
+    <t>答案（正确/错误）</t>
+  </si>
+  <si>
+    <t>小鱼很喜欢我</t>
+  </si>
+  <si>
+    <t>正确</t>
   </si>
   <si>
     <t>选项A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>选项B</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>选项C</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>选项D</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>答案</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>答案（正确/错误）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>表格测试</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>小鱼姓什么</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>姓王！</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>小鱼很喜欢我</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>正确</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>小鱼小鱼</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>咕嘟嘟</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>哗啦啦</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>噼里啪啦</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>CHARMING</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>D</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -125,14 +90,13 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="新細明體"/>
-      <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="新細明體"/>
-      <family val="2"/>
+      <family val="1"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
@@ -223,7 +187,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -256,26 +220,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -308,23 +255,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -467,23 +397,18 @@
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F501CF02-8FC3-3247-B233-C6F9FB760ADB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
@@ -493,18 +418,18 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -514,14 +439,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59F746AF-9B99-0A49-99E0-11905DF85494}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="17.83203125" customWidth="1"/>
   </cols>
@@ -534,18 +459,18 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -555,14 +480,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAF40DC8-D6A1-5746-A1C0-A8CDDFAEAAB6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
@@ -572,24 +497,24 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
some bug for import; svg show
</commit_message>
<xml_diff>
--- a/src/main/resources/static/import_temp/template.xlsx
+++ b/src/main/resources/static/import_temp/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/23Fall/JAVA/finalProj/KaskadeMindBank/src/main/resources/static/import_temp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D32F3C-CFAA-9245-A509-5A0A9BF66516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A9E85A-0AE4-9C41-93B8-95DFD0FFFB3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2960" yWindow="660" windowWidth="22500" windowHeight="13700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4140" yWindow="660" windowWidth="22500" windowHeight="13700" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fill" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>主题</t>
   </si>
@@ -33,24 +33,9 @@
     <t>答案</t>
   </si>
   <si>
-    <t>表格测试</t>
-  </si>
-  <si>
-    <t>小鱼姓什么</t>
-  </si>
-  <si>
-    <t>姓王！</t>
-  </si>
-  <si>
     <t>答案（正确/错误）</t>
   </si>
   <si>
-    <t>小鱼很喜欢我</t>
-  </si>
-  <si>
-    <t>正确</t>
-  </si>
-  <si>
     <t>选项A</t>
   </si>
   <si>
@@ -63,29 +48,39 @@
     <t>选项D</t>
   </si>
   <si>
-    <t>小鱼小鱼</t>
-  </si>
-  <si>
-    <t>咕嘟嘟</t>
-  </si>
-  <si>
-    <t>哗啦啦</t>
-  </si>
-  <si>
-    <t>噼里啪啦</t>
-  </si>
-  <si>
-    <t>CHARMING</t>
+    <t>1+1=</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>判断测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>填空测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1+1=4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>错误</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>选择测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -95,6 +90,14 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="新細明體"/>
       <family val="1"/>
       <charset val="136"/>
@@ -123,8 +126,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -404,8 +410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15"/>
@@ -422,14 +428,14 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -443,7 +449,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15"/>
@@ -459,18 +465,18 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -483,8 +489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15"/>
@@ -497,42 +503,42 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="G2" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>